<commit_message>
Corrección: columna NOMBRE_EPS en EPS.xlsx
</commit_message>
<xml_diff>
--- a/EPS.xlsx
+++ b/EPS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonProyectos\CallCenter_Limpio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CCDD99C-C367-49EC-9BC5-8AAA69D68EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3128C25F-B8E4-4FBB-8BF1-01820A83618B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C64F12D0-32B2-45CD-A086-79F63D5CF8D4}"/>
   </bookViews>
@@ -36,12 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="365">
   <si>
-    <t>CODIGO_EPS</t>
-  </si>
-  <si>
-    <t>NOMBRE_EPS</t>
-  </si>
-  <si>
     <t>EPS001</t>
   </si>
   <si>
@@ -1129,6 +1123,12 @@
   </si>
   <si>
     <t>BAVARIA</t>
+  </si>
+  <si>
+    <t>Nombre_EPS</t>
+  </si>
+  <si>
+    <t>Codigo_EPS</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1209,7 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1219,8 +1219,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1537,9 +1537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44998690-BB5C-478B-98A3-EE3420BEC6A3}">
   <dimension ref="A1:R214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1548,18 +1546,18 @@
   <sheetData>
     <row r="1" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>0</v>
+        <v>364</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>1</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1580,10 +1578,10 @@
     </row>
     <row r="3" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1604,10 +1602,10 @@
     </row>
     <row r="4" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1628,10 +1626,10 @@
     </row>
     <row r="5" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1652,10 +1650,10 @@
     </row>
     <row r="6" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1676,10 +1674,10 @@
     </row>
     <row r="7" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1700,10 +1698,10 @@
     </row>
     <row r="8" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1724,10 +1722,10 @@
     </row>
     <row r="9" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1748,10 +1746,10 @@
     </row>
     <row r="10" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1772,10 +1770,10 @@
     </row>
     <row r="11" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1796,10 +1794,10 @@
     </row>
     <row r="12" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1820,10 +1818,10 @@
     </row>
     <row r="13" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1844,10 +1842,10 @@
     </row>
     <row r="14" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1868,10 +1866,10 @@
     </row>
     <row r="15" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1892,10 +1890,10 @@
     </row>
     <row r="16" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1916,10 +1914,10 @@
     </row>
     <row r="17" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1940,10 +1938,10 @@
     </row>
     <row r="18" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1964,10 +1962,10 @@
     </row>
     <row r="19" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1988,10 +1986,10 @@
     </row>
     <row r="20" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -2012,10 +2010,10 @@
     </row>
     <row r="21" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -2036,10 +2034,10 @@
     </row>
     <row r="22" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -2060,10 +2058,10 @@
     </row>
     <row r="23" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -2084,10 +2082,10 @@
     </row>
     <row r="24" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -2108,10 +2106,10 @@
     </row>
     <row r="25" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -2132,10 +2130,10 @@
     </row>
     <row r="26" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -2156,10 +2154,10 @@
     </row>
     <row r="27" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -2180,10 +2178,10 @@
     </row>
     <row r="28" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -2204,10 +2202,10 @@
     </row>
     <row r="29" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -2228,10 +2226,10 @@
     </row>
     <row r="30" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -2252,10 +2250,10 @@
     </row>
     <row r="31" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -2276,10 +2274,10 @@
     </row>
     <row r="32" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -2300,10 +2298,10 @@
     </row>
     <row r="33" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -2324,10 +2322,10 @@
     </row>
     <row r="34" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -2348,10 +2346,10 @@
     </row>
     <row r="35" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -2372,10 +2370,10 @@
     </row>
     <row r="36" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -2396,10 +2394,10 @@
     </row>
     <row r="37" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -2420,10 +2418,10 @@
     </row>
     <row r="38" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -2444,10 +2442,10 @@
     </row>
     <row r="39" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -2468,10 +2466,10 @@
     </row>
     <row r="40" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -2492,10 +2490,10 @@
     </row>
     <row r="41" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -2516,10 +2514,10 @@
     </row>
     <row r="42" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -2540,10 +2538,10 @@
     </row>
     <row r="43" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -2564,10 +2562,10 @@
     </row>
     <row r="44" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -2588,10 +2586,10 @@
     </row>
     <row r="45" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -2612,10 +2610,10 @@
     </row>
     <row r="46" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -2636,10 +2634,10 @@
     </row>
     <row r="47" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -2660,10 +2658,10 @@
     </row>
     <row r="48" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -2684,10 +2682,10 @@
     </row>
     <row r="49" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -2708,10 +2706,10 @@
     </row>
     <row r="50" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -2732,10 +2730,10 @@
     </row>
     <row r="51" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -2756,10 +2754,10 @@
     </row>
     <row r="52" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -2780,10 +2778,10 @@
     </row>
     <row r="53" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -2804,10 +2802,10 @@
     </row>
     <row r="54" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -2828,10 +2826,10 @@
     </row>
     <row r="55" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -2852,10 +2850,10 @@
     </row>
     <row r="56" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -2876,10 +2874,10 @@
     </row>
     <row r="57" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -2900,10 +2898,10 @@
     </row>
     <row r="58" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -2924,10 +2922,10 @@
     </row>
     <row r="59" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -2948,10 +2946,10 @@
     </row>
     <row r="60" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -2972,10 +2970,10 @@
     </row>
     <row r="61" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -2996,10 +2994,10 @@
     </row>
     <row r="62" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -3020,10 +3018,10 @@
     </row>
     <row r="63" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -3044,10 +3042,10 @@
     </row>
     <row r="64" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -3068,10 +3066,10 @@
     </row>
     <row r="65" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -3092,10 +3090,10 @@
     </row>
     <row r="66" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -3116,10 +3114,10 @@
     </row>
     <row r="67" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -3140,10 +3138,10 @@
     </row>
     <row r="68" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -3164,10 +3162,10 @@
     </row>
     <row r="69" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -3188,10 +3186,10 @@
     </row>
     <row r="70" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -3212,10 +3210,10 @@
     </row>
     <row r="71" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
@@ -3236,10 +3234,10 @@
     </row>
     <row r="72" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
@@ -3260,10 +3258,10 @@
     </row>
     <row r="73" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
@@ -3284,10 +3282,10 @@
     </row>
     <row r="74" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
@@ -3308,10 +3306,10 @@
     </row>
     <row r="75" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
@@ -3332,10 +3330,10 @@
     </row>
     <row r="76" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
@@ -3356,10 +3354,10 @@
     </row>
     <row r="77" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
@@ -3380,10 +3378,10 @@
     </row>
     <row r="78" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
@@ -3404,10 +3402,10 @@
     </row>
     <row r="79" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
@@ -3428,10 +3426,10 @@
     </row>
     <row r="80" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
@@ -3452,10 +3450,10 @@
     </row>
     <row r="81" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
@@ -3476,10 +3474,10 @@
     </row>
     <row r="82" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
@@ -3500,10 +3498,10 @@
     </row>
     <row r="83" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
@@ -3524,10 +3522,10 @@
     </row>
     <row r="84" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
@@ -3548,10 +3546,10 @@
     </row>
     <row r="85" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
@@ -3572,10 +3570,10 @@
     </row>
     <row r="86" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
@@ -3596,10 +3594,10 @@
     </row>
     <row r="87" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
@@ -3620,10 +3618,10 @@
     </row>
     <row r="88" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
@@ -3644,10 +3642,10 @@
     </row>
     <row r="89" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
@@ -3668,10 +3666,10 @@
     </row>
     <row r="90" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
@@ -3692,10 +3690,10 @@
     </row>
     <row r="91" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
@@ -3716,10 +3714,10 @@
     </row>
     <row r="92" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
@@ -3740,10 +3738,10 @@
     </row>
     <row r="93" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
@@ -3764,10 +3762,10 @@
     </row>
     <row r="94" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
@@ -3788,10 +3786,10 @@
     </row>
     <row r="95" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
@@ -3812,10 +3810,10 @@
     </row>
     <row r="96" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
@@ -3836,10 +3834,10 @@
     </row>
     <row r="97" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
@@ -3860,10 +3858,10 @@
     </row>
     <row r="98" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
@@ -3884,10 +3882,10 @@
     </row>
     <row r="99" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
@@ -3908,10 +3906,10 @@
     </row>
     <row r="100" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
@@ -3932,10 +3930,10 @@
     </row>
     <row r="101" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
@@ -3956,10 +3954,10 @@
     </row>
     <row r="102" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
@@ -3980,10 +3978,10 @@
     </row>
     <row r="103" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
@@ -4004,10 +4002,10 @@
     </row>
     <row r="104" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
@@ -4028,10 +4026,10 @@
     </row>
     <row r="105" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
@@ -4052,10 +4050,10 @@
     </row>
     <row r="106" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
@@ -4076,10 +4074,10 @@
     </row>
     <row r="107" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
@@ -4100,10 +4098,10 @@
     </row>
     <row r="108" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
@@ -4124,10 +4122,10 @@
     </row>
     <row r="109" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
@@ -4148,10 +4146,10 @@
     </row>
     <row r="110" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
@@ -4172,10 +4170,10 @@
     </row>
     <row r="111" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
@@ -4196,10 +4194,10 @@
     </row>
     <row r="112" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
@@ -4220,10 +4218,10 @@
     </row>
     <row r="113" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
@@ -4244,10 +4242,10 @@
     </row>
     <row r="114" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
@@ -4268,10 +4266,10 @@
     </row>
     <row r="115" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
@@ -4292,10 +4290,10 @@
     </row>
     <row r="116" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C116" s="3"/>
       <c r="D116" s="3"/>
@@ -4316,10 +4314,10 @@
     </row>
     <row r="117" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
@@ -4340,10 +4338,10 @@
     </row>
     <row r="118" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
@@ -4367,7 +4365,7 @@
         <v>36904</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
@@ -4391,7 +4389,7 @@
         <v>37024</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
@@ -4415,7 +4413,7 @@
         <v>37055</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
@@ -4439,7 +4437,7 @@
         <v>37085</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
@@ -4463,7 +4461,7 @@
         <v>37116</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
@@ -4487,7 +4485,7 @@
         <v>37147</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
@@ -4511,7 +4509,7 @@
         <v>37177</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
@@ -4535,7 +4533,7 @@
         <v>37238</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
@@ -4556,10 +4554,10 @@
     </row>
     <row r="127" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
@@ -4580,10 +4578,10 @@
     </row>
     <row r="128" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
@@ -4604,10 +4602,10 @@
     </row>
     <row r="129" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
@@ -4628,10 +4626,10 @@
     </row>
     <row r="130" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C130" s="3"/>
       <c r="D130" s="3"/>
@@ -4652,10 +4650,10 @@
     </row>
     <row r="131" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C131" s="3"/>
       <c r="D131" s="3"/>
@@ -4676,10 +4674,10 @@
     </row>
     <row r="132" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C132" s="3"/>
       <c r="D132" s="3"/>
@@ -4700,10 +4698,10 @@
     </row>
     <row r="133" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C133" s="3"/>
       <c r="D133" s="3"/>
@@ -4724,10 +4722,10 @@
     </row>
     <row r="134" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
@@ -4748,10 +4746,10 @@
     </row>
     <row r="135" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C135" s="3"/>
       <c r="D135" s="3"/>
@@ -4772,10 +4770,10 @@
     </row>
     <row r="136" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
@@ -4796,10 +4794,10 @@
     </row>
     <row r="137" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C137" s="3"/>
       <c r="D137" s="3"/>
@@ -4820,10 +4818,10 @@
     </row>
     <row r="138" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C138" s="3"/>
       <c r="D138" s="3"/>
@@ -4844,10 +4842,10 @@
     </row>
     <row r="139" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C139" s="3"/>
       <c r="D139" s="3"/>
@@ -4868,10 +4866,10 @@
     </row>
     <row r="140" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C140" s="3"/>
       <c r="D140" s="3"/>
@@ -4892,10 +4890,10 @@
     </row>
     <row r="141" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C141" s="3"/>
       <c r="D141" s="3"/>
@@ -4916,10 +4914,10 @@
     </row>
     <row r="142" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C142" s="3"/>
       <c r="D142" s="3"/>
@@ -4940,10 +4938,10 @@
     </row>
     <row r="143" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
@@ -4967,7 +4965,7 @@
         <v>36905</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
@@ -4991,7 +4989,7 @@
         <v>36995</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C145" s="3"/>
       <c r="D145" s="3"/>
@@ -5015,7 +5013,7 @@
         <v>37025</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C146" s="3"/>
       <c r="D146" s="3"/>
@@ -5039,7 +5037,7 @@
         <v>37086</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
@@ -5063,7 +5061,7 @@
         <v>37117</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C148" s="3"/>
       <c r="D148" s="3"/>
@@ -5087,7 +5085,7 @@
         <v>37148</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C149" s="3"/>
       <c r="D149" s="3"/>
@@ -5111,7 +5109,7 @@
         <v>37178</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
@@ -5135,7 +5133,7 @@
         <v>37209</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C151" s="3"/>
       <c r="D151" s="3"/>
@@ -5156,10 +5154,10 @@
     </row>
     <row r="152" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
@@ -5180,10 +5178,10 @@
     </row>
     <row r="153" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C153" s="3"/>
       <c r="D153" s="3"/>
@@ -5204,10 +5202,10 @@
     </row>
     <row r="154" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C154" s="3"/>
       <c r="D154" s="3"/>
@@ -5228,10 +5226,10 @@
     </row>
     <row r="155" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C155" s="3"/>
       <c r="D155" s="3"/>
@@ -5252,10 +5250,10 @@
     </row>
     <row r="156" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C156" s="3"/>
       <c r="D156" s="3"/>
@@ -5276,10 +5274,10 @@
     </row>
     <row r="157" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C157" s="3"/>
       <c r="D157" s="3"/>
@@ -5300,10 +5298,10 @@
     </row>
     <row r="158" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
@@ -5324,10 +5322,10 @@
     </row>
     <row r="159" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C159" s="3"/>
       <c r="D159" s="3"/>
@@ -5348,10 +5346,10 @@
     </row>
     <row r="160" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C160" s="3"/>
       <c r="D160" s="3"/>
@@ -5372,10 +5370,10 @@
     </row>
     <row r="161" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C161" s="3"/>
       <c r="D161" s="3"/>
@@ -5396,10 +5394,10 @@
     </row>
     <row r="162" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C162" s="3"/>
       <c r="D162" s="3"/>
@@ -5420,10 +5418,10 @@
     </row>
     <row r="163" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C163" s="3"/>
       <c r="D163" s="3"/>
@@ -5444,10 +5442,10 @@
     </row>
     <row r="164" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C164" s="3"/>
       <c r="D164" s="3"/>
@@ -5468,10 +5466,10 @@
     </row>
     <row r="165" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C165" s="3"/>
       <c r="D165" s="3"/>
@@ -5492,10 +5490,10 @@
     </row>
     <row r="166" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C166" s="3"/>
       <c r="D166" s="3"/>
@@ -5519,7 +5517,7 @@
         <v>36906</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C167" s="3"/>
       <c r="D167" s="3"/>
@@ -5543,7 +5541,7 @@
         <v>36937</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C168" s="3"/>
       <c r="D168" s="3"/>
@@ -5567,7 +5565,7 @@
         <v>5000</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C169" s="3"/>
       <c r="D169" s="3"/>
@@ -5591,7 +5589,7 @@
         <v>8000</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C170" s="3"/>
       <c r="D170" s="3"/>
@@ -5615,7 +5613,7 @@
         <v>11001</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C171" s="3"/>
       <c r="D171" s="3"/>
@@ -5639,7 +5637,7 @@
         <v>13000</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C172" s="3"/>
       <c r="D172" s="3"/>
@@ -5663,7 +5661,7 @@
         <v>15000</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C173" s="3"/>
       <c r="D173" s="3"/>
@@ -5687,7 +5685,7 @@
         <v>17000</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C174" s="3"/>
       <c r="D174" s="3"/>
@@ -5711,7 +5709,7 @@
         <v>18000</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C175" s="3"/>
       <c r="D175" s="3"/>
@@ -5735,7 +5733,7 @@
         <v>19000</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C176" s="3"/>
       <c r="D176" s="3"/>
@@ -5759,7 +5757,7 @@
         <v>20000</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C177" s="3"/>
       <c r="D177" s="3"/>
@@ -5783,7 +5781,7 @@
         <v>23000</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C178" s="3"/>
       <c r="D178" s="3"/>
@@ -5807,7 +5805,7 @@
         <v>25000</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C179" s="3"/>
       <c r="D179" s="3"/>
@@ -5831,7 +5829,7 @@
         <v>27000</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C180" s="3"/>
       <c r="D180" s="3"/>
@@ -5855,7 +5853,7 @@
         <v>41000</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C181" s="3"/>
       <c r="D181" s="3"/>
@@ -5879,7 +5877,7 @@
         <v>44000</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C182" s="3"/>
       <c r="D182" s="3"/>
@@ -5903,7 +5901,7 @@
         <v>47000</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C183" s="3"/>
       <c r="D183" s="3"/>
@@ -5927,7 +5925,7 @@
         <v>50000</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C184" s="3"/>
       <c r="D184" s="3"/>
@@ -5951,7 +5949,7 @@
         <v>52000</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C185" s="3"/>
       <c r="D185" s="3"/>
@@ -5975,7 +5973,7 @@
         <v>54000</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C186" s="3"/>
       <c r="D186" s="3"/>
@@ -5999,7 +5997,7 @@
         <v>63000</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C187" s="3"/>
       <c r="D187" s="3"/>
@@ -6023,7 +6021,7 @@
         <v>66000</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C188" s="3"/>
       <c r="D188" s="3"/>
@@ -6047,7 +6045,7 @@
         <v>68000</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C189" s="3"/>
       <c r="D189" s="3"/>
@@ -6071,7 +6069,7 @@
         <v>70000</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C190" s="3"/>
       <c r="D190" s="3"/>
@@ -6095,7 +6093,7 @@
         <v>73000</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C191" s="3"/>
       <c r="D191" s="3"/>
@@ -6119,7 +6117,7 @@
         <v>76000</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C192" s="3"/>
       <c r="D192" s="3"/>
@@ -6143,7 +6141,7 @@
         <v>81000</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C193" s="3"/>
       <c r="D193" s="3"/>
@@ -6167,7 +6165,7 @@
         <v>85000</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C194" s="3"/>
       <c r="D194" s="3"/>
@@ -6191,7 +6189,7 @@
         <v>86000</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C195" s="3"/>
       <c r="D195" s="3"/>
@@ -6215,7 +6213,7 @@
         <v>88000</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C196" s="3"/>
       <c r="D196" s="3"/>
@@ -6239,7 +6237,7 @@
         <v>91000</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C197" s="3"/>
       <c r="D197" s="3"/>
@@ -6263,7 +6261,7 @@
         <v>94000</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C198" s="3"/>
       <c r="D198" s="3"/>
@@ -6287,7 +6285,7 @@
         <v>95000</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C199" s="3"/>
       <c r="D199" s="3"/>
@@ -6311,7 +6309,7 @@
         <v>97000</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C200" s="3"/>
       <c r="D200" s="3"/>
@@ -6335,7 +6333,7 @@
         <v>99000</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C201" s="3"/>
       <c r="D201" s="3"/>
@@ -6356,10 +6354,10 @@
     </row>
     <row r="202" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C202" s="3"/>
       <c r="D202" s="3"/>
@@ -6380,10 +6378,10 @@
     </row>
     <row r="203" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C203" s="3"/>
       <c r="D203" s="3"/>
@@ -6404,10 +6402,10 @@
     </row>
     <row r="204" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C204" s="3"/>
       <c r="D204" s="3"/>
@@ -6428,10 +6426,10 @@
     </row>
     <row r="205" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C205" s="3"/>
       <c r="D205" s="3"/>
@@ -6452,10 +6450,10 @@
     </row>
     <row r="206" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C206" s="3"/>
       <c r="D206" s="3"/>
@@ -6476,10 +6474,10 @@
     </row>
     <row r="207" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C207" s="3"/>
       <c r="D207" s="3"/>
@@ -6500,10 +6498,10 @@
     </row>
     <row r="208" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C208" s="3"/>
       <c r="D208" s="3"/>
@@ -6524,10 +6522,10 @@
     </row>
     <row r="209" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C209" s="3"/>
       <c r="D209" s="3"/>
@@ -6548,10 +6546,10 @@
     </row>
     <row r="210" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C210" s="3"/>
       <c r="D210" s="3"/>
@@ -6572,10 +6570,10 @@
     </row>
     <row r="211" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C211" s="3"/>
       <c r="D211" s="3"/>
@@ -6596,10 +6594,10 @@
     </row>
     <row r="212" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C212" s="3"/>
       <c r="D212" s="3"/>
@@ -6620,10 +6618,10 @@
     </row>
     <row r="213" spans="1:18" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C213" s="3"/>
       <c r="D213" s="3"/>
@@ -6644,10 +6642,10 @@
     </row>
     <row r="214" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A214" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C214" s="5"/>
       <c r="D214" s="5"/>

</xml_diff>